<commit_message>
Added shared formulas in Excel
</commit_message>
<xml_diff>
--- a/data/extracted.xlsx
+++ b/data/extracted.xlsx
@@ -4,10 +4,39 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Oh, sheet" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Oh, sheet" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>ORgo Ciald</t>
+  </si>
+  <si>
+    <t>Ciadk voj</t>
+  </si>
+  <si>
+    <t>Diavolo a 4</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,18 +411,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1">
-        <f>A1 / B1</f>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D5" si="0">C2 * A2</f>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
       </c>
     </row>
   </sheetData>

</xml_diff>